<commit_message>
Stand up the NSantiam simulation. Add another 2 sections to the Handbook. CW3MdigitalHandbook.docx - Add sections on first principles model and tuning knobs. NSantiam/flow2010.ic - From Baseline_2000-09_C166. Flow_NSantiam.xml - Get the flow reports working.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -1,34 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M\trunk\DataCW3M\RegressionTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F4F87D-282D-496E-A169-3177FE31C653}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F707A3BF-41C4-422D-87ED-9404329EB99A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27315" windowHeight="15945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="6" r:id="rId1"/>
     <sheet name="2010-17" sheetId="5" r:id="rId2"/>
-    <sheet name="CW3M c118 2010" sheetId="1" r:id="rId3"/>
-    <sheet name="CW3M c106 2010" sheetId="4" r:id="rId4"/>
-    <sheet name="INFEWS demo 0.3.2_Nov9" sheetId="2" r:id="rId5"/>
+    <sheet name="2010-18" sheetId="7" r:id="rId3"/>
+    <sheet name="CW3M c118 2010" sheetId="1" r:id="rId4"/>
+    <sheet name="CW3M c106 2010" sheetId="4" r:id="rId5"/>
+    <sheet name="INFEWS demo 0.3.2_Nov9" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'CW3M c106 2010'!$A$1:$O$2</definedName>
-    <definedName name="ExternalData_1" localSheetId="4" hidden="1">'INFEWS demo 0.3.2_Nov9'!$A$1:$O$2</definedName>
+    <definedName name="ExternalData_1" localSheetId="4" hidden="1">'CW3M c106 2010'!$A$1:$O$2</definedName>
+    <definedName name="ExternalData_1" localSheetId="5" hidden="1">'INFEWS demo 0.3.2_Nov9'!$A$1:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -50,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="54">
   <si>
     <t>Year</t>
   </si>
@@ -188,6 +192,30 @@
   </si>
   <si>
     <t>new multiyear baseline climate; irrigation?</t>
+  </si>
+  <si>
+    <t>avg 2010-17</t>
+  </si>
+  <si>
+    <t>Baseline_2010-18_C166</t>
+  </si>
+  <si>
+    <t>CW3M github</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> water added by FlowModel (mm)</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>simulation run</t>
+  </si>
+  <si>
+    <t>weather years</t>
+  </si>
+  <si>
+    <t>2010-18</t>
   </si>
 </sst>
 </file>
@@ -692,7 +720,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -726,6 +754,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1183,14 +1217,14 @@
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>2010</v>
       </c>
@@ -1237,7 +1271,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -1284,7 +1318,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1365,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -1378,7 +1412,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -1425,7 +1459,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>26</v>
       </c>
@@ -1472,7 +1506,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1522,7 +1556,7 @@
         <v>-1.9380000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1575,7 +1609,7 @@
         <v>-2.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1628,7 +1662,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>42</v>
       </c>
@@ -1684,7 +1718,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1700,7 +1734,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1750,7 +1784,7 @@
         <v>-4.9200000000000003E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -1797,7 +1831,7 @@
         <v>2.6899999999999998E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -1844,7 +1878,7 @@
         <v>-1.3799999999999999E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1891,7 +1925,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>24</v>
       </c>
@@ -1938,7 +1972,7 @@
         <v>-1.725E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1954,7 +1988,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1970,7 +2004,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -2017,7 +2051,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2077,23 +2111,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{484B6A0E-51A6-4D53-B3C5-495F7D5D6E35}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD26"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="7" customWidth="1"/>
-    <col min="4" max="13" width="9.140625" style="3"/>
-    <col min="14" max="15" width="9.140625" style="5"/>
-    <col min="17" max="17" width="9.140625" style="4"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="7" customWidth="1"/>
+    <col min="4" max="9" width="9.109375" style="3"/>
+    <col min="10" max="10" width="8.88671875" style="3"/>
+    <col min="11" max="14" width="9.109375" style="3"/>
+    <col min="15" max="16" width="9.109375" style="5"/>
+    <col min="18" max="18" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>2010</v>
       </c>
@@ -2119,31 +2155,34 @@
         <v>6</v>
       </c>
       <c r="J1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -2165,32 +2204,32 @@
       <c r="I2" s="3">
         <v>0</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>619.16601600000001</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>106.250168</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>1611.582275</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="3">
         <v>1112.4111330000001</v>
       </c>
-      <c r="N2" s="5">
+      <c r="O2" s="5">
         <v>5408.5908200000003</v>
       </c>
-      <c r="O2" s="5">
+      <c r="P2" s="5">
         <v>2338.7646479999999</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>-6.1512269999999996</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -2212,32 +2251,32 @@
       <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="8">
+      <c r="K3" s="8">
         <v>619.16601600000001</v>
       </c>
-      <c r="K3" s="8">
+      <c r="L3" s="8">
         <v>106.250168</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>1611.582764</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>1112.4107670000001</v>
       </c>
-      <c r="N3" s="9">
+      <c r="O3" s="9">
         <v>5408.609375</v>
       </c>
-      <c r="O3" s="9">
+      <c r="P3" s="9">
         <v>2338.7646479999999</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>-6.1511050000000003</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="R3" s="10">
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -2259,32 +2298,32 @@
       <c r="I4" s="3">
         <v>0</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>619.16601600000001</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>106.250168</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>1611.582764</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>1112.4107670000001</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>5408.609375</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>2338.7646479999999</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>-6.1511050000000003</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="R4" s="4">
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -2306,32 +2345,32 @@
       <c r="I5" s="3">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>619.16601600000001</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>106.250168</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>1611.5832519999999</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="3">
         <v>1112.4105219999999</v>
       </c>
-      <c r="N5" s="5">
+      <c r="O5" s="5">
         <v>5408.609375</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="5">
         <v>2338.7646479999999</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>-6.1508609999999999</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="R5" s="4">
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2359,96 +2398,105 @@
       <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>605.89157112500004</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>98.322234500000022</v>
       </c>
-      <c r="L6" s="8">
+      <c r="M6" s="8">
         <v>1670.4636995000001</v>
       </c>
-      <c r="M6" s="3">
+      <c r="N6" s="3">
         <v>687.16619875000004</v>
       </c>
-      <c r="N6" s="11">
+      <c r="O6" s="11">
         <v>14850.296875</v>
       </c>
-      <c r="O6" s="5">
+      <c r="P6" s="5">
         <v>2220.293823125</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>-0.12632575000000013</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="R6" s="4">
         <v>-2.2962500000000007E-4</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="7" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="22">
+        <v>668.5519142500001</v>
+      </c>
+      <c r="E7" s="22">
+        <v>2156.1590268749997</v>
+      </c>
+      <c r="F7" s="22">
+        <v>5.6243153749999992</v>
+      </c>
+      <c r="G7" s="22">
+        <v>190.44139825000002</v>
+      </c>
+      <c r="H7" s="22">
+        <v>0</v>
+      </c>
+      <c r="I7" s="22">
+        <v>1.2914638750000003</v>
+      </c>
+      <c r="J7" s="22">
+        <v>0</v>
+      </c>
+      <c r="K7" s="22">
+        <v>608.64128874999994</v>
+      </c>
+      <c r="L7" s="22">
+        <v>99.615801250000004</v>
+      </c>
+      <c r="M7" s="22">
+        <v>1637.9830476250002</v>
+      </c>
+      <c r="N7" s="22">
+        <v>675.73597337499996</v>
+      </c>
+      <c r="O7" s="23">
+        <v>14924.480468624999</v>
+      </c>
+      <c r="P7" s="23">
+        <v>2220.293823125</v>
+      </c>
+      <c r="Q7" s="22">
+        <v>-9.2008500000000132E-2</v>
+      </c>
+      <c r="R7" s="24">
+        <v>-7.2000000000000029E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1099.9311520000001</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2191.751221</v>
-      </c>
-      <c r="F8" s="3">
-        <v>2.2251270000000001</v>
-      </c>
-      <c r="G8" s="8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>775.43878199999995</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <v>1608.7592770000001</v>
-      </c>
-      <c r="M8" s="3">
-        <v>1099.2677000000001</v>
-      </c>
-      <c r="N8" s="5">
-        <v>5390.8964839999999</v>
-      </c>
-      <c r="O8" s="5">
-        <v>2010.6401370000001</v>
-      </c>
-      <c r="P8" s="2">
-        <v>189.558258</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>5.7548000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="3">
         <v>1099.9311520000001</v>
       </c>
       <c r="E9" s="3">
-        <v>2182.702393</v>
+        <v>2191.751221</v>
       </c>
       <c r="F9" s="3">
-        <v>2.1869450000000001</v>
-      </c>
-      <c r="G9" s="3">
-        <v>190.31104999999999</v>
+        <v>2.2251270000000001</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
       </c>
       <c r="H9" s="3">
         <v>0</v>
@@ -2456,43 +2504,43 @@
       <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9" s="3">
-        <v>843.08422900000005</v>
-      </c>
       <c r="K9" s="3">
-        <v>0</v>
+        <v>775.43878199999995</v>
       </c>
       <c r="L9" s="3">
-        <v>1384.994751</v>
+        <v>0</v>
       </c>
       <c r="M9" s="3">
-        <v>1247.9868160000001</v>
-      </c>
-      <c r="N9" s="5">
-        <v>6436.2304690000001</v>
+        <v>1608.7592770000001</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1099.2677000000001</v>
       </c>
       <c r="O9" s="5">
+        <v>5390.8964839999999</v>
+      </c>
+      <c r="P9" s="5">
         <v>2010.6401370000001</v>
       </c>
-      <c r="P9">
-        <v>0.93425599999999998</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>2.6899999999999998E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q9" s="2">
+        <v>189.558258</v>
+      </c>
+      <c r="R9" s="10">
+        <v>5.7548000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3">
         <v>1099.9311520000001</v>
       </c>
       <c r="E10" s="3">
-        <v>2197.9660640000002</v>
+        <v>2182.702393</v>
       </c>
       <c r="F10" s="3">
-        <v>2.2625820000000001</v>
+        <v>2.1869450000000001</v>
       </c>
       <c r="G10" s="3">
         <v>190.31104999999999</v>
@@ -2503,79 +2551,79 @@
       <c r="I10" s="3">
         <v>0</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
+        <v>843.08422900000005</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1384.994751</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1247.9868160000001</v>
+      </c>
+      <c r="O10" s="5">
+        <v>6436.2304690000001</v>
+      </c>
+      <c r="P10" s="5">
+        <v>2010.6401370000001</v>
+      </c>
+      <c r="Q10">
+        <v>0.93425599999999998</v>
+      </c>
+      <c r="R10" s="4">
+        <v>2.6899999999999998E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1099.9311520000001</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2197.9660640000002</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2.2625820000000001</v>
+      </c>
+      <c r="G11" s="3">
+        <v>190.31104999999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
         <v>840.81152299999997</v>
       </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3">
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
         <v>1410.530884</v>
       </c>
-      <c r="M10" s="3">
+      <c r="N11" s="3">
         <v>1238.64624</v>
       </c>
-      <c r="N10" s="5">
+      <c r="O11" s="5">
         <v>6658.3554690000001</v>
       </c>
-      <c r="O10" s="5">
+      <c r="P11" s="5">
         <v>2010.6401370000001</v>
       </c>
-      <c r="P10">
+      <c r="Q11">
         <v>-0.48220200000000002</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="R11" s="4">
         <v>-1.3799999999999999E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>2010</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1071.1062010000001</v>
-      </c>
-      <c r="E12" s="3">
-        <v>2191.751221</v>
-      </c>
-      <c r="F12" s="3">
-        <v>2.391721</v>
-      </c>
-      <c r="G12" s="3">
-        <v>190.31167600000001</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0</v>
-      </c>
-      <c r="J12" s="3">
-        <v>619.16601600000001</v>
-      </c>
-      <c r="K12" s="3">
-        <v>106.250168</v>
-      </c>
-      <c r="L12" s="3">
-        <v>1611.5832519999999</v>
-      </c>
-      <c r="M12" s="3">
-        <v>1112.4105219999999</v>
-      </c>
-      <c r="N12" s="5">
-        <v>5408.609375</v>
-      </c>
-      <c r="O12" s="5">
-        <v>2338.7646479999999</v>
-      </c>
-      <c r="P12">
-        <v>-6.1508609999999999</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>-1.7799999999999999E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2010</v>
       </c>
@@ -2597,81 +2645,81 @@
       <c r="I13" s="3">
         <v>0</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>619.16601600000001</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>106.250168</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <v>1611.5832519999999</v>
       </c>
-      <c r="M13" s="3">
+      <c r="N13" s="3">
         <v>1112.4105219999999</v>
       </c>
-      <c r="N13" s="5">
+      <c r="O13" s="5">
         <v>5408.609375</v>
       </c>
-      <c r="O13" s="5">
+      <c r="P13" s="5">
         <v>2338.7646479999999</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>-6.1508609999999999</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="R13" s="4">
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>2010</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1071.1062010000001</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2191.751221</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2.391721</v>
+      </c>
+      <c r="G14" s="3">
+        <v>190.31167600000001</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>619.16601600000001</v>
+      </c>
+      <c r="L14" s="3">
+        <v>106.250168</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1611.5832519999999</v>
+      </c>
+      <c r="N14" s="3">
+        <v>1112.4105219999999</v>
+      </c>
+      <c r="O14" s="5">
+        <v>5408.609375</v>
+      </c>
+      <c r="P14" s="5">
+        <v>2338.7646479999999</v>
+      </c>
+      <c r="Q14">
+        <v>-6.1508609999999999</v>
+      </c>
+      <c r="R14" s="4">
+        <v>-1.7799999999999999E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>22</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1078.9810790000001</v>
-      </c>
-      <c r="E15" s="3">
-        <v>2163.12571725</v>
-      </c>
-      <c r="F15" s="3">
-        <v>2.7222486250000002</v>
-      </c>
-      <c r="G15" s="3">
-        <v>190.31167600000001</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0</v>
-      </c>
-      <c r="J15" s="3">
-        <v>589.4486236250001</v>
-      </c>
-      <c r="K15" s="3">
-        <v>97.848918499999996</v>
-      </c>
-      <c r="L15" s="3">
-        <v>1673.5501557499999</v>
-      </c>
-      <c r="M15" s="3">
-        <v>1072.836235</v>
-      </c>
-      <c r="N15" s="5">
-        <v>6562.1458129999992</v>
-      </c>
-      <c r="O15" s="5">
-        <v>2219.0386962499997</v>
-      </c>
-      <c r="P15" s="3">
-        <v>-1.4567878749999998</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>-5.2175000000000008E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>23</v>
       </c>
       <c r="D16" s="3">
         <v>1078.9810790000001</v>
@@ -2691,187 +2739,234 @@
       <c r="I16" s="3">
         <v>0</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <v>589.4486236250001</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L16" s="3">
         <v>97.848918499999996</v>
       </c>
-      <c r="L16" s="3">
+      <c r="M16" s="3">
         <v>1673.5501557499999</v>
       </c>
-      <c r="M16" s="3">
+      <c r="N16" s="3">
         <v>1072.836235</v>
       </c>
-      <c r="N16" s="5">
+      <c r="O16" s="5">
         <v>6562.1458129999992</v>
       </c>
-      <c r="O16" s="5">
+      <c r="P16" s="5">
         <v>2219.0386962499997</v>
       </c>
-      <c r="P16" s="3">
+      <c r="Q16" s="3">
         <v>-1.4567878749999998</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="R16" s="4">
         <v>-5.2175000000000008E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1078.9810790000001</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2163.12571725</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2.7222486250000002</v>
+      </c>
+      <c r="G17" s="3">
+        <v>190.31167600000001</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>589.4486236250001</v>
+      </c>
+      <c r="L17" s="3">
+        <v>97.848918499999996</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1673.5501557499999</v>
+      </c>
+      <c r="N17" s="3">
+        <v>1072.836235</v>
+      </c>
+      <c r="O17" s="5">
+        <v>6562.1458129999992</v>
+      </c>
+      <c r="P17" s="5">
+        <v>2219.0386962499997</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>-1.4567878749999998</v>
+      </c>
+      <c r="R17" s="4">
+        <v>-5.2175000000000008E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D18" s="3">
         <v>1058.044563125</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E18" s="3">
         <v>2100.9735717499998</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F18" s="3">
         <v>2.7169057500000005</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G18" s="3">
         <v>187.70465100000001</v>
       </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0</v>
-      </c>
-      <c r="J17" s="3">
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
         <v>583.40168787500011</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L18" s="3">
         <v>93.776032874999999</v>
       </c>
-      <c r="L17" s="3">
+      <c r="M18" s="3">
         <v>1622.8268737500002</v>
       </c>
-      <c r="M17" s="3">
+      <c r="N18" s="3">
         <v>1049.18328075</v>
       </c>
-      <c r="N17" s="5">
+      <c r="O18" s="5">
         <v>6561.7244262499989</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P18" s="5">
         <v>2193.7870484999999</v>
       </c>
-      <c r="P17" s="3">
+      <c r="Q18" s="3">
         <v>-0.25181649999999989</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="R18" s="4">
         <v>-1.1250000000000009E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="P18" s="3"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D20" s="3">
         <v>1078.9810790000001</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E20" s="3">
         <v>2163.12571725</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F20" s="3">
         <v>2.7222486250000002</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G20" s="3">
         <v>190.31167600000001</v>
       </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0</v>
-      </c>
-      <c r="J19" s="3">
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
         <v>589.4486236250001</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L20" s="3">
         <v>97.848918499999996</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M20" s="3">
         <v>1673.5501557499999</v>
       </c>
-      <c r="M19" s="3">
+      <c r="N20" s="3">
         <v>1072.836235</v>
       </c>
-      <c r="N19" s="5">
+      <c r="O20" s="5">
         <v>6562.1458129999992</v>
       </c>
-      <c r="O19" s="5">
+      <c r="P20" s="5">
         <v>2219.0386962499997</v>
       </c>
-      <c r="P19" s="3">
+      <c r="Q20" s="3">
         <v>-1.4567878749999998</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="R20" s="4">
         <v>-5.2175000000000008E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D22" s="3">
         <v>1064.4662779999999</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E22" s="3">
         <v>2159.8282013749999</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F22" s="3">
         <v>2.6925776250000002</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G22" s="3">
         <v>190.31167600000001</v>
       </c>
-      <c r="H21" s="3">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0</v>
-      </c>
-      <c r="J21" s="8">
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8">
         <v>727.62358862499991</v>
       </c>
-      <c r="K21" s="3">
-        <v>0</v>
-      </c>
-      <c r="L21" s="8">
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="8">
         <v>1604.030212375</v>
       </c>
-      <c r="M21" s="3">
+      <c r="N22" s="3">
         <v>1085.9620207499997</v>
       </c>
-      <c r="N21" s="9">
+      <c r="O22" s="9">
         <v>6300.5065918749997</v>
       </c>
-      <c r="O21" s="9">
+      <c r="P22" s="9">
         <v>2085.5385894999999</v>
       </c>
-      <c r="P21" s="3">
+      <c r="Q22" s="3">
         <v>0.31708862499999957</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="R22" s="10">
         <v>-4.8124999999999882E-5</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S22" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2881,6 +2976,143 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="3">
+        <v>665.2496372222223</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2102.3245847777775</v>
+      </c>
+      <c r="F2" s="3">
+        <v>5.805838333333333</v>
+      </c>
+      <c r="G2" s="3">
+        <v>190.42691511111113</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.3487368888888891</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>592.70844188888884</v>
+      </c>
+      <c r="L2" s="3">
+        <v>97.826613000000009</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1604.4250625555558</v>
+      </c>
+      <c r="N2" s="3">
+        <v>670.26834788888891</v>
+      </c>
+      <c r="O2" s="5">
+        <v>15521.784071111111</v>
+      </c>
+      <c r="P2" s="5">
+        <v>2216.7525497777779</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>7.2752111111111004E-2</v>
+      </c>
+      <c r="R2" s="4">
+        <v>-2.4444444444444675E-6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
@@ -2888,12 +3120,12 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>2010</v>
       </c>
@@ -2940,7 +3172,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2987,7 +3219,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -3034,7 +3266,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3086,7 +3318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EDEF300-F934-4EE5-B044-F2D97979A2C5}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -3094,26 +3326,26 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3160,7 +3392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -3215,7 +3447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -3223,26 +3455,26 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3289,7 +3521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010</v>
       </c>

</xml_diff>

<commit_message>
Release CW3M_Installer_McKenzie_0.4.3.exe. McKenzie stream flows and temperatures have been calibrated to USGS gage data for 2010-18.  Special logic was added for the springs which feed Clear Lake.  The special logic provides for a constant spring flow of 5.7 cms plus a seasonally-varying additional spring flow of 0.8351 times the amount simulated as flowing into Clear from upstream.  The Demo and Baseline scenarios have been combined into a single Demo_Baseline scenario.  This release includes files for the Clackamas and North Santiam basins as well as for the McKenzie.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F707A3BF-41C4-422D-87ED-9404329EB99A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA5FEF9-2C1E-43ED-B121-080CC12ADB42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="6" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="55">
   <si>
     <t>Year</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>2010-18</t>
+  </si>
+  <si>
+    <t>Baseline_2010-18_C205</t>
   </si>
 </sst>
 </file>
@@ -2977,16 +2980,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
@@ -3104,6 +3108,65 @@
         <v>-2.4444444444444675E-6</v>
       </c>
       <c r="S2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="3">
+        <v>677.32165200000009</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F3" s="3">
+        <v>5.6902922222222223</v>
+      </c>
+      <c r="G3" s="3">
+        <v>190.42691511111113</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.321501777777778</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>566.90397822222212</v>
+      </c>
+      <c r="L3" s="3">
+        <v>96.602825555555569</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1624.5496012222222</v>
+      </c>
+      <c r="N3" s="3">
+        <v>681.18569955555552</v>
+      </c>
+      <c r="O3" s="9">
+        <v>15160.787543444445</v>
+      </c>
+      <c r="P3" s="5">
+        <v>2216.7525497777779</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0.18215544444444445</v>
+      </c>
+      <c r="R3" s="4">
+        <v>-4.5222222222222227E-5</v>
+      </c>
+      <c r="S3" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit code changes for spinup mode. These haven't been tested yet. HBV.csv - Add names for Mehama37 and LowerNSantiam44. EnvContext.h - Add EnvContext::spinupFlag. EnvLoader.cpp - Add "spinup" field to <settings> block. Flow.cpp, .h - Add spinupFlag as an argument to ReadState() and ResetStateVariables(). Overhaul ReadState() to add spinup logic.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D16374B-74F5-452F-9EEC-ACC8EAC37518}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F36C79B-3A8C-43BB-8CF8-93C5E2B72176}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="57">
   <si>
     <t>Year</t>
   </si>
@@ -221,7 +221,10 @@
     <t>Baseline_2010-18_C205</t>
   </si>
   <si>
-    <t>Baseline 2010-18 C267+</t>
+    <t>Baseline 2010-18 C369</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C367+</t>
   </si>
 </sst>
 </file>
@@ -2986,7 +2989,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3178,7 +3181,7 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>53</v>
@@ -3230,21 +3233,60 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="4"/>
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="3">
+        <v>677.97837322222222</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4.820043222222222</v>
+      </c>
+      <c r="G5" s="3">
+        <v>232.21855144444442</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>6.3389989999999994</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>586.02156566666656</v>
+      </c>
+      <c r="L5" s="3">
+        <v>96.631732222222212</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1650.8734266666665</v>
+      </c>
+      <c r="N5" s="3">
+        <v>682.41798233333327</v>
+      </c>
+      <c r="O5" s="9">
+        <v>12820.605631666667</v>
+      </c>
+      <c r="P5" s="5">
+        <v>2216.7525497777779</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.28915188888888882</v>
+      </c>
+      <c r="R5" s="4">
+        <v>-2.4444444444444798E-6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
I think spinup mode is working now. This version has a new spinup for NSantiam. NSantiam/flow2010.ic - from spinning up over 2000-09 HRU_NSantiam.dbf, IDU_NSantiam.dbf, Reach_NSantiam.dbf - As at the end of the spinup. Flow.cpp - Fix a typo.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F36C79B-3A8C-43BB-8CF8-93C5E2B72176}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E2AE94-A05A-4352-AF0F-569B7E520642}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="58">
   <si>
     <t>Year</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C367+</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C371+</t>
   </si>
 </sst>
 </file>
@@ -2986,10 +2989,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3286,6 +3289,62 @@
       </c>
       <c r="R5" s="4">
         <v>-2.4444444444444798E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="3">
+        <v>675.83090190000007</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2040.5741823000001</v>
+      </c>
+      <c r="F6" s="8">
+        <v>5.7945578999999992</v>
+      </c>
+      <c r="G6" s="3">
+        <v>232.20442180000001</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>6.2224744999999997</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>549.56830450000007</v>
+      </c>
+      <c r="L6" s="8">
+        <v>86.997628399999996</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1652.2535766000001</v>
+      </c>
+      <c r="N6" s="8">
+        <v>668.55730879999999</v>
+      </c>
+      <c r="O6" s="9">
+        <v>15727.597461100002</v>
+      </c>
+      <c r="P6" s="5">
+        <v>2215.5502928999999</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>-3.2497201000000002</v>
+      </c>
+      <c r="R6" s="4">
+        <v>-1.3625999999999998E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust for the difference between gage drainage areas and HBVCALIB areas at 5 gages in NSantiam. Flow.xml - Increase the Boulder Creek spring flow by 60 cfs to get the summer minimum flows right. Turn off the Blowout Cr spring. Reduce the Breitenbush spring from 159 cfs to 20 cfs to get the summer minimum flows right. HBV.csv - Reduce ET_MULT for LittleNSantiam50 from 1.0 to 0.1. FLOWreports_NSantiam.xml - Add factors to adjust for the difference between gage drainage areas and HBVCALIB areas (from HBVCALIBandGages_NSantiam.xlsx) for 5 drainages: Blowout Cr, NSantiam at Niagara, Little NSantiam near Mehama, NSantiam at Mehama, and NSantiam at Greens Bridge. Flow.cpp - Remove an obsolete comment.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276D45FA-AC23-4CA8-9268-F52083508C49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0D2BEF-B381-4C48-A42C-020D96519D4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="60">
   <si>
     <t>Year</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C374</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C377+</t>
   </si>
 </sst>
 </file>
@@ -2992,10 +2995,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3404,6 +3407,62 @@
       </c>
       <c r="R7" s="4">
         <v>-1.0888888888888886E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="8">
+        <v>686.88716633333343</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5.8066811111111116</v>
+      </c>
+      <c r="G8" s="3">
+        <v>190.76777833333335</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>5.9919669999999989</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>535.46594233333337</v>
+      </c>
+      <c r="L8" s="3">
+        <v>89.974237444444441</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1665.6726211111111</v>
+      </c>
+      <c r="N8" s="8">
+        <v>692.90829122222226</v>
+      </c>
+      <c r="O8" s="5">
+        <v>15597.417643111112</v>
+      </c>
+      <c r="P8" s="5">
+        <v>2216.8192002222222</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.26791133333333339</v>
+      </c>
+      <c r="R8" s="4">
+        <v>-1.1666666666666722E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get PEST_Blowout51 working. CW3M_PEST_Blowout51.envx - Add spinup='0'. Flow_PEST.xml - Turn on NSantiam springs as in Flow.xml. PEST_Blowout51/flow2010.ic, HRU_PEST_Blowout51.dbf, IDU_PEST_Blowout51.dbf, Reach_PEST_Blowout51.dbf - From spinup over 2000-09.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B660716-104E-4F7A-A5E5-3EE22BF43DCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12523AA1-9D2F-4761-A7CE-EE36F820C6E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,7 @@
     <definedName name="ExternalData_1" localSheetId="5" hidden="1">'INFEWS demo 0.3.2_Nov9'!$A$1:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="62">
   <si>
     <t>Year</t>
   </si>
@@ -237,6 +238,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C379</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C381</t>
   </si>
 </sst>
 </file>
@@ -2998,10 +3002,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3522,6 +3526,62 @@
       </c>
       <c r="R9" s="4">
         <v>7.7777777777776053E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3">
+        <v>684.40618233333328</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F10" s="3">
+        <v>5.8168283333333335</v>
+      </c>
+      <c r="G10" s="3">
+        <v>195.47808666666668</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>6.0423557777777779</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>539.90315411111123</v>
+      </c>
+      <c r="L10" s="3">
+        <v>92.016936222222228</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1664.2275663333335</v>
+      </c>
+      <c r="N10" s="3">
+        <v>690.17001011111108</v>
+      </c>
+      <c r="O10" s="5">
+        <v>15526.62749577778</v>
+      </c>
+      <c r="P10" s="5">
+        <v>2216.8192002222222</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0.27462577777777786</v>
+      </c>
+      <c r="R10" s="4">
+        <v>-8.5555555555556067E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Release CW3M_McKenzie 0.4.13. SimulationScenarios_PEST.xml - Comment out PEST_Spinup. CW3M_McKenzie_Script.iss - Change revision from 0.4.12 to 0.4.13.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12523AA1-9D2F-4761-A7CE-EE36F820C6E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BAE7FE-1D39-48FF-BA88-A29BA74D03E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="37380" yWindow="-1260" windowWidth="11670" windowHeight="5400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <definedName name="ExternalData_1" localSheetId="5" hidden="1">'INFEWS demo 0.3.2_Nov9'!$A$1:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="63">
   <si>
     <t>Year</t>
   </si>
@@ -241,6 +240,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C381</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C389</t>
   </si>
 </sst>
 </file>
@@ -3002,10 +3004,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3582,6 +3584,62 @@
       </c>
       <c r="R10" s="4">
         <v>-8.5555555555556067E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3">
+        <v>677.93100322222222</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F11" s="3">
+        <v>5.8089704444444443</v>
+      </c>
+      <c r="G11" s="3">
+        <v>195.47808666666668</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>6.060794111111111</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>540.71662055555544</v>
+      </c>
+      <c r="L11" s="3">
+        <v>91.777595333333338</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1663.296996888889</v>
+      </c>
+      <c r="N11" s="3">
+        <v>684.06924111111107</v>
+      </c>
+      <c r="O11" s="9">
+        <v>15695.633789222222</v>
+      </c>
+      <c r="P11" s="5">
+        <v>2216.8192002222222</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0.28201211111111113</v>
+      </c>
+      <c r="R11" s="4">
+        <v>-5.7777777777777738E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flow.xml and Flow_PEST.xml - Turn on the spring on Blowout Cr. at 8 cfs. Add a Breitenbush Hot Spring at 0.42 cfs but 84 deg C. HBV.csv - Apply David Holman's new PEST calibrations for Blowout51, LittleNSantiam50, and DET12. FLOWreports_PEST_Blowout51.xml - Use new observation data files from Observations/Willamette Gages/Flow.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BAE7FE-1D39-48FF-BA88-A29BA74D03E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF674EB-0E83-4BD2-A54D-48E4F8A9C661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="37380" yWindow="-1260" windowWidth="11670" windowHeight="5400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="6" r:id="rId1"/>
     <sheet name="2010-17" sheetId="5" r:id="rId2"/>
     <sheet name="2010-18" sheetId="7" r:id="rId3"/>
-    <sheet name="CW3M c118 2010" sheetId="1" r:id="rId4"/>
-    <sheet name="CW3M c106 2010" sheetId="4" r:id="rId5"/>
-    <sheet name="INFEWS demo 0.3.2_Nov9" sheetId="2" r:id="rId6"/>
+    <sheet name="2000-09 spinup" sheetId="8" r:id="rId4"/>
+    <sheet name="CW3M c118 2010" sheetId="1" r:id="rId5"/>
+    <sheet name="CW3M c106 2010" sheetId="4" r:id="rId6"/>
+    <sheet name="INFEWS demo 0.3.2_Nov9" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="4" hidden="1">'CW3M c106 2010'!$A$1:$O$2</definedName>
-    <definedName name="ExternalData_1" localSheetId="5" hidden="1">'INFEWS demo 0.3.2_Nov9'!$A$1:$O$2</definedName>
+    <definedName name="ExternalData_1" localSheetId="5" hidden="1">'CW3M c106 2010'!$A$1:$O$2</definedName>
+    <definedName name="ExternalData_1" localSheetId="6" hidden="1">'INFEWS demo 0.3.2_Nov9'!$A$1:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="67">
   <si>
     <t>Year</t>
   </si>
@@ -243,6 +244,18 @@
   </si>
   <si>
     <t>Baseline 2010-18 C389</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C393</t>
+  </si>
+  <si>
+    <t>2000-09</t>
+  </si>
+  <si>
+    <t>Baseline 2000-09 5/9/21 spinup</t>
+  </si>
+  <si>
+    <t>Baseline 2000-09 C393 spinup</t>
   </si>
 </sst>
 </file>
@@ -3004,10 +3017,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3642,12 +3655,257 @@
         <v>-5.7777777777777738E-6</v>
       </c>
     </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3">
+        <v>677.93100322222222</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5.8089704444444443</v>
+      </c>
+      <c r="G12" s="3">
+        <v>195.47808666666668</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>6.060794111111111</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>540.71662055555544</v>
+      </c>
+      <c r="L12" s="3">
+        <v>91.777595333333338</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1663.296996888889</v>
+      </c>
+      <c r="N12" s="3">
+        <v>684.06924111111107</v>
+      </c>
+      <c r="O12" s="5">
+        <v>15695.633789222222</v>
+      </c>
+      <c r="P12" s="5">
+        <v>2216.8192002222222</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0.28201211111111113</v>
+      </c>
+      <c r="R12" s="4">
+        <v>-5.7777777777777738E-6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBF95DE-E389-464A-AFAF-011155A18B88}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="3">
+        <v>572.4274934</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1951.2097047</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6.0977103000000001</v>
+      </c>
+      <c r="G2" s="3">
+        <v>195.51971589999999</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>7.3807704000000003</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>545.82672409999998</v>
+      </c>
+      <c r="L2" s="3">
+        <v>92.905869899999999</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1490.1102661999998</v>
+      </c>
+      <c r="N2" s="3">
+        <v>603.64529430000005</v>
+      </c>
+      <c r="O2" s="5">
+        <v>16485.282812500001</v>
+      </c>
+      <c r="P2" s="5">
+        <v>1985.1201415999999</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>-0.14723959999999991</v>
+      </c>
+      <c r="R2" s="4">
+        <v>-3.2939999999999998E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3">
+        <v>571.75505380000004</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1951.2097047</v>
+      </c>
+      <c r="F3" s="3">
+        <v>5.8274805000000001</v>
+      </c>
+      <c r="G3" s="3">
+        <v>195.51971589999999</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>7.3943439999999994</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>545.72043469999994</v>
+      </c>
+      <c r="L3" s="3">
+        <v>93.221763699999997</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1489.4764649000001</v>
+      </c>
+      <c r="N3" s="3">
+        <v>603.14073799999994</v>
+      </c>
+      <c r="O3" s="9">
+        <v>15579.5007324</v>
+      </c>
+      <c r="P3" s="5">
+        <v>1985.1201415999999</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>-0.14689749999999976</v>
+      </c>
+      <c r="R3" s="4">
+        <v>-3.3019999999999989E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
@@ -3853,7 +4111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EDEF300-F934-4EE5-B044-F2D97979A2C5}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -3982,7 +4240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>

</xml_diff>

<commit_message>
HBV.csv - Incorporate new PEST calibration values for GreensBr44 (aka LowerNSantiam). FLOWreports_NSantiam.xml - Add a yearly report, "FLOW NSantiam Water Budget". Reporter_NSantiam.xml and Reporter.xml - Add a report, "REP NSantiam water budget". FLOWreports_PEST_GreensBr44.xml - Add columns for upstream gages to monthly FLOW Q_DISCHARG at gage report. FLOWreports_WRB.xml - Add FLOW WRB-NSantiam Water Budget report. Add FLOW WRB-NSantiam flow skill assessment monthly report.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF674EB-0E83-4BD2-A54D-48E4F8A9C661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67F15F4-C314-4FFB-BA86-05B02BB26AF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="6" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="69">
   <si>
     <t>Year</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>Baseline 2000-09 C393 spinup</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C402</t>
+  </si>
+  <si>
+    <t>added 174 cfs spring in the Little Nsantiam basin</t>
   </si>
 </sst>
 </file>
@@ -760,7 +766,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -800,6 +806,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3017,10 +3024,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3030,7 +3037,7 @@
     <col min="18" max="18" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -3089,7 +3096,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -3148,7 +3155,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -3207,7 +3214,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3263,7 +3270,7 @@
         <v>-2.4444444444444798E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -3319,7 +3326,7 @@
         <v>-2.4444444444444798E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -3375,7 +3382,7 @@
         <v>-1.3625999999999998E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3431,7 +3438,7 @@
         <v>-1.0888888888888886E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -3487,7 +3494,7 @@
         <v>-1.1666666666666722E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3543,7 +3550,7 @@
         <v>7.7777777777776053E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -3599,7 +3606,7 @@
         <v>-8.5555555555556067E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -3655,7 +3662,7 @@
         <v>-5.7777777777777738E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3711,8 +3718,68 @@
         <v>-5.7777777777777738E-6</v>
       </c>
     </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="8">
+        <v>529.14105211111109</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1.6230948888888888</v>
+      </c>
+      <c r="G13" s="8">
+        <v>332.2750817777777</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>7.3481075555555559</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>520.64759333333336</v>
+      </c>
+      <c r="L13" s="3">
+        <v>91.777595333333338</v>
+      </c>
+      <c r="M13" s="8">
+        <v>1836.442098</v>
+      </c>
+      <c r="N13" s="8">
+        <v>515.86576666666667</v>
+      </c>
+      <c r="O13" s="25">
+        <v>3819.0314398888886</v>
+      </c>
+      <c r="P13" s="5">
+        <v>2216.8192002222222</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>4.6129111111111114E-2</v>
+      </c>
+      <c r="R13" s="10">
+        <v>-1.0222222222222218E-5</v>
+      </c>
+      <c r="T13" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3720,7 +3787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBF95DE-E389-464A-AFAF-011155A18B88}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Continue to add calibration and skill assessment information to the sections on the McKenzie and North Santiam basins in the CW3M Digital Handbook.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67F15F4-C314-4FFB-BA86-05B02BB26AF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC3F1CE-836B-4CAF-A1BC-82B96B57CDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="6" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="71">
   <si>
     <t>Year</t>
   </si>
@@ -262,14 +262,21 @@
   </si>
   <si>
     <t>added 174 cfs spring in the Little Nsantiam basin</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C409</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> weather years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -722,7 +729,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -765,8 +772,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -807,8 +815,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -848,6 +861,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -3024,16 +3038,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3044,56 +3059,56 @@
       <c r="B1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
-        <v>52</v>
+      <c r="S1" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -3775,6 +3790,220 @@
       </c>
       <c r="T13" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="3">
+        <v>538.14217811111109</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F14" s="8">
+        <v>6.3960675555555557</v>
+      </c>
+      <c r="G14" s="3">
+        <v>332.2750817777777</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>8.1963734444444434</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="8">
+        <v>596.58821288888896</v>
+      </c>
+      <c r="L14" s="3">
+        <v>91.777595333333338</v>
+      </c>
+      <c r="M14" s="8">
+        <v>1766.6258951111113</v>
+      </c>
+      <c r="N14" s="8">
+        <v>524.36296266666659</v>
+      </c>
+      <c r="O14" s="9">
+        <v>16731.370117222221</v>
+      </c>
+      <c r="P14" s="5">
+        <v>2216.8192002222222</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>4.5377222222222208E-2</v>
+      </c>
+      <c r="R14" s="4">
+        <v>-9.2222222222222292E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D15" s="3"/>
+      <c r="E15" s="26">
+        <f>E14/$E17</f>
+        <v>0.85790914466193569</v>
+      </c>
+      <c r="F15" s="27">
+        <f>(F14)/$E17</f>
+        <v>2.6200859120246106E-3</v>
+      </c>
+      <c r="G15" s="26">
+        <f>G14/$E17</f>
+        <v>0.13611320598491744</v>
+      </c>
+      <c r="H15" s="27">
+        <f>H14/$E17</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="26">
+        <f>I14/$E17</f>
+        <v>3.3575634411222542E-3</v>
+      </c>
+      <c r="J15" s="26">
+        <f>J14/$E14</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="26">
+        <f t="shared" ref="K15:M15" si="0">K14/$E14</f>
+        <v>0.28486288033426305</v>
+      </c>
+      <c r="L15" s="26">
+        <f t="shared" si="0"/>
+        <v>4.3822572407535863E-2</v>
+      </c>
+      <c r="M15" s="26">
+        <f t="shared" si="0"/>
+        <v>0.84354020089929849</v>
+      </c>
+      <c r="N15" s="3">
+        <f>N14-D14</f>
+        <v>-13.779215444444503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D16" s="3"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28">
+        <f>(G14*1898320000/1000)/(365.25*24*60*60)</f>
+        <v>19.987718750487712</v>
+      </c>
+      <c r="H16" s="27"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26">
+        <f>J14/$M14</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="26">
+        <f t="shared" ref="K16:M16" si="1">K14/$M14</f>
+        <v>0.33769923476150948</v>
+      </c>
+      <c r="L16" s="26">
+        <f t="shared" si="1"/>
+        <v>5.1950781196695307E-2</v>
+      </c>
+      <c r="M16" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N16" s="28">
+        <f>N15/9</f>
+        <v>-1.5310239382716115</v>
+      </c>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <f>SUM(E14:I14)</f>
+        <v>2441.1671106666663</v>
+      </c>
+      <c r="F17" s="26">
+        <f>F15+H15</f>
+        <v>2.6200859120246106E-3</v>
+      </c>
+      <c r="G17" s="29">
+        <f>G14/M14</f>
+        <v>0.18808457562934081</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3">
+        <f>SUM(J14:M14)</f>
+        <v>2454.9917033333336</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3">
+        <f>(M14/1000)*1898320000/(365.25*24*60*60)</f>
+        <v>106.26984527363693</v>
+      </c>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="26">
+        <f>J17/E14</f>
+        <v>1.1722256536410975</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="28">
+        <f>J17-E17</f>
+        <v>13.824592666667286</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="27">
+        <f>J19/E17</f>
+        <v>5.6631078660124515E-3</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="J21" s="3">
+        <f>J19-N16</f>
+        <v>15.355616604938897</v>
+      </c>
+    </row>
+    <row r="22" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="J22" s="30">
+        <f>J21/E14</f>
+        <v>7.332101239831584E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stand up the SchaferCreek52 study area. Add CW3M_PEST_SchaferCreek52.envx Add the PEST_SchaferCreek52 folder, with IDU, HRU, and Reach shapefiles, flow2010.ic, and a FLOWreports XML file. Flow.cpp - Add code to handle 2 places where subtracting nominally equal numbers yields tiny negative results instead of 0.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC3F1CE-836B-4CAF-A1BC-82B96B57CDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A380E2-9C10-4422-BCD6-8D99896AD252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="6" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="72">
   <si>
     <t>Year</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t xml:space="preserve"> weather years</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C445</t>
   </si>
 </sst>
 </file>
@@ -3038,10 +3041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3922,7 +3925,7 @@
         <v>-1.5310239382716115</v>
       </c>
     </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
       <c r="E17" s="3">
         <f>SUM(E14:I14)</f>
@@ -3949,7 +3952,7 @@
         <v>106.26984527363693</v>
       </c>
     </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="26"/>
@@ -3964,7 +3967,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="26"/>
@@ -3979,7 +3982,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="26"/>
@@ -3994,16 +3997,72 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J21" s="3">
         <f>J19-N16</f>
         <v>15.355616604938897</v>
       </c>
     </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J22" s="30">
         <f>J21/E14</f>
         <v>7.332101239831584E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="3">
+        <v>538.12494244444451</v>
+      </c>
+      <c r="E24" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F24" s="3">
+        <v>5.8220211111111109</v>
+      </c>
+      <c r="G24" s="3">
+        <v>332.2750817777777</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>8.1971097777777775</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <v>596.67409588888893</v>
+      </c>
+      <c r="L24" s="3">
+        <v>91.777595333333338</v>
+      </c>
+      <c r="M24" s="3">
+        <v>1765.9676106666668</v>
+      </c>
+      <c r="N24" s="3">
+        <v>524.34534722222224</v>
+      </c>
+      <c r="O24" s="9">
+        <v>15018.345052222223</v>
+      </c>
+      <c r="P24" s="5">
+        <v>2216.8192002222222</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>4.5906222222222182E-2</v>
+      </c>
+      <c r="R24" s="4">
+        <v>-8.9999999999999901E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start to catch up on log entries on changes made since version 502. The next commit will have some more log entries for these changes. lulc.xml - Add class 62221 PABFdrying. EnvDoc.cpp - Add logic to OpenDocXml() to return the value that LoadProject() returns when the value is < 1. Envision.cpp - Refine an error message. wetland_deterministic_transition_lookup.csv, wetland_probabilistic_transition_lookup.csv - Remove unneeded columns and reorder the remaining columns. IDU_McKenzie.dbf, IDU_NSantiam.dbf - Add WET_FRAC. WetlandSTM.xml - Remove unneeded fields. CW3M.sln - Add STMengine to the DEBUG configuration.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_NSantiam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5759035-77E2-4520-88C4-14DCB4BC2AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDD078E-38A7-4C1B-947C-24E85CA2B01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="6" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="79">
   <si>
     <t>Year</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C502</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C549</t>
   </si>
 </sst>
 </file>
@@ -1300,14 +1303,14 @@
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>2010</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>26</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>-1.9380000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1692,7 +1695,7 @@
         <v>-2.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>42</v>
       </c>
@@ -1801,7 +1804,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1817,7 +1820,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>-4.9200000000000003E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -1914,7 +1917,7 @@
         <v>2.6899999999999998E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -1961,7 +1964,7 @@
         <v>-1.3799999999999999E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -2008,7 +2011,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>24</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>-1.725E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -2071,7 +2074,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2087,7 +2090,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -2134,7 +2137,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2200,19 +2203,19 @@
       <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="7" customWidth="1"/>
-    <col min="4" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="8.85546875" style="3"/>
-    <col min="11" max="14" width="9.140625" style="3"/>
-    <col min="15" max="16" width="9.140625" style="5"/>
-    <col min="18" max="18" width="9.140625" style="4"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="7" customWidth="1"/>
+    <col min="4" max="9" width="9.109375" style="3"/>
+    <col min="10" max="10" width="8.88671875" style="3"/>
+    <col min="11" max="14" width="9.109375" style="3"/>
+    <col min="15" max="16" width="9.109375" style="5"/>
+    <col min="18" max="18" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>2010</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -2406,7 +2409,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -2453,7 +2456,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2509,7 +2512,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>48</v>
       </c>
@@ -2565,7 +2568,7 @@
         <v>-7.2000000000000029E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>5.7548000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>2.6899999999999998E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -2706,7 +2709,7 @@
         <v>-1.3799999999999999E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2010</v>
       </c>
@@ -2753,7 +2756,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2010</v>
       </c>
@@ -2800,7 +2803,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -2847,7 +2850,7 @@
         <v>-5.2175000000000008E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>-5.2175000000000008E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>25</v>
       </c>
@@ -2941,10 +2944,10 @@
         <v>-1.1250000000000009E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>-5.2175000000000008E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -3060,24 +3063,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98986-E186-479F-9224-9914F025E666}">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="10" ySplit="6" topLeftCell="K16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -3136,7 +3139,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -3195,7 +3198,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -3254,7 +3257,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>-2.4444444444444798E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>-2.4444444444444798E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -3422,7 +3425,7 @@
         <v>-1.3625999999999998E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3478,7 +3481,7 @@
         <v>-1.0888888888888886E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -3534,7 +3537,7 @@
         <v>-1.1666666666666722E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3590,7 +3593,7 @@
         <v>7.7777777777776053E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -3646,7 +3649,7 @@
         <v>-8.5555555555556067E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -3702,7 +3705,7 @@
         <v>-5.7777777777777738E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3758,7 +3761,7 @@
         <v>-5.7777777777777738E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3873,7 +3876,7 @@
         <v>-9.2222222222222292E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D15" s="3"/>
       <c r="E15" s="26">
         <f>E14/$E17</f>
@@ -3916,7 +3919,7 @@
         <v>-13.779215444444503</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
       <c r="E16" s="26"/>
       <c r="F16" s="27"/>
@@ -3947,7 +3950,7 @@
         <v>-1.5310239382716115</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
       <c r="E17" s="3">
         <f>SUM(E14:I14)</f>
@@ -3974,7 +3977,7 @@
         <v>106.26984527363693</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="26"/>
@@ -3989,7 +3992,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -4045,7 +4048,7 @@
         <v>-8.5555555555555711E-6</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -4101,7 +4104,7 @@
         <v>-8.5555555555555711E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -4157,19 +4160,19 @@
         <v>3.1555555555555551E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J22" s="3">
         <f>J19-N16</f>
         <v>1.5310239382716115</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J23" s="30">
         <f>J22/E14</f>
         <v>7.3104342240497007E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -4225,7 +4228,7 @@
         <v>-8.9999999999999901E-6</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -4281,7 +4284,7 @@
         <v>-8.3333333333333439E-6</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -4337,7 +4340,7 @@
         <v>-8.5555555555555711E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -4393,7 +4396,7 @@
         <v>3.1555555555555551E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -4449,7 +4452,7 @@
         <v>3.1555555555555551E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -4502,6 +4505,62 @@
         <v>0.15968566666666667</v>
       </c>
       <c r="R30" s="4">
+        <v>3.1444444444444436E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="3">
+        <v>500.77147766666673</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2094.2995878888887</v>
+      </c>
+      <c r="F31" s="3">
+        <v>6.3999523333333332</v>
+      </c>
+      <c r="G31" s="3">
+        <v>332.2750817777777</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8.7763246666666657</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
+        <v>596.69084999999995</v>
+      </c>
+      <c r="L31" s="3">
+        <v>92.364316777777788</v>
+      </c>
+      <c r="M31" s="3">
+        <v>1750.163886111111</v>
+      </c>
+      <c r="N31" s="3">
+        <v>503.4630568888889</v>
+      </c>
+      <c r="O31" s="5">
+        <v>16172.367621555555</v>
+      </c>
+      <c r="P31" s="5">
+        <v>2216.8192002222222</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0.15968566666666667</v>
+      </c>
+      <c r="R31" s="4">
         <v>3.1444444444444436E-5</v>
       </c>
     </row>
@@ -4519,12 +4578,12 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -4583,7 +4642,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -4639,7 +4698,7 @@
         <v>-3.2939999999999998E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4708,12 +4767,12 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>2010</v>
       </c>
@@ -4760,7 +4819,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -4807,7 +4866,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -4854,7 +4913,7 @@
         <v>-1.7799999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4914,26 +4973,26 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4980,7 +5039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -5043,26 +5102,26 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5109,7 +5168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010</v>
       </c>

</xml_diff>